<commit_message>
add sync salesman & term, add schedule
</commit_message>
<xml_diff>
--- a/public/file/autonic.xlsx
+++ b/public/file/autonic.xlsx
@@ -16,12 +16,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Kode Barang</t>
   </si>
   <si>
     <t>Stok</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Satuan</t>
+  </si>
+  <si>
+    <t>Laptop 1</t>
+  </si>
+  <si>
+    <t>Mouse 1</t>
+  </si>
+  <si>
+    <t>Keyboard 1</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>10004S</t>
+  </si>
+  <si>
+    <t>10003S</t>
+  </si>
+  <si>
+    <t>10001S</t>
   </si>
 </sst>
 </file>
@@ -360,44 +387,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10004</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10003</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10001</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>